<commit_message>
rework of category model - adding period and details fields, removing category field
</commit_message>
<xml_diff>
--- a/fileloader/file.xlsx
+++ b/fileloader/file.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="25">
   <si>
     <t xml:space="preserve">Text</t>
   </si>
@@ -28,10 +28,13 @@
     <t xml:space="preserve">Answer</t>
   </si>
   <si>
-    <t xml:space="preserve">Category</t>
-  </si>
-  <si>
-    <t xml:space="preserve">answer_type</t>
+    <t xml:space="preserve">Period</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Answer_type</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Details</t>
   </si>
   <si>
     <t xml:space="preserve">W których latach toczyła się pierwsza wojna punicka?</t>
@@ -46,6 +49,9 @@
     <t xml:space="preserve">przedział czasowy roczny</t>
   </si>
   <si>
+    <t xml:space="preserve">republika rzymska</t>
+  </si>
+  <si>
     <t xml:space="preserve">W których latach toczyła się druga wojna punicka?</t>
   </si>
   <si>
@@ -79,37 +85,16 @@
     <t xml:space="preserve">202 p.n.e.</t>
   </si>
   <si>
-    <t xml:space="preserve">W którym roku odbyła się bitwa pod Maratonem?</t>
-  </si>
-  <si>
-    <t xml:space="preserve">490 p.n.e.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">W których latach toczyła się druga wojna perska?</t>
-  </si>
-  <si>
-    <t xml:space="preserve">480 – 449 p.n.e.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">W którym roku odbyła się bitwa pod Cheroneą?</t>
-  </si>
-  <si>
-    <t xml:space="preserve">338 p.n.e.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">W którym roku odbyła się bitwa pod Rafią?</t>
+    <t xml:space="preserve">W którym roku odbyła się bitwa nad Jeziorem Trazymeńskim?</t>
   </si>
   <si>
     <t xml:space="preserve">217 p.n.e.</t>
   </si>
   <si>
-    <t xml:space="preserve">W których latach panował Antioch III Wielki, władca Seleucydów?</t>
-  </si>
-  <si>
-    <t xml:space="preserve">223 – 187 p.n.e.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">W którym roku odbyła się bitwa nad Jeziorem Trazymeńskim?</t>
+    <t xml:space="preserve">W których latach toczyła się pierwsza wojna macedońska?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">215 p.n.e. – 205 p.n.e.</t>
   </si>
 </sst>
 </file>
@@ -119,26 +104,36 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="4">
+  <fonts count="5">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
       <name val="Arial"/>
       <family val="0"/>
+      <charset val="238"/>
     </font>
     <font>
       <sz val="10"/>
       <name val="Arial"/>
       <family val="0"/>
+      <charset val="238"/>
     </font>
     <font>
       <sz val="10"/>
       <name val="Arial"/>
       <family val="0"/>
+      <charset val="238"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="238"/>
     </font>
   </fonts>
   <fills count="2">
@@ -183,8 +178,12 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -205,18 +204,19 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:D13"/>
+  <dimension ref="A1:E9"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D14" activeCellId="0" sqref="D14"/>
+      <selection pane="topLeft" activeCell="A13" activeCellId="0" sqref="A13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="63.36"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="30.28"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="23.89"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="63.37"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="22.89"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="23.88"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="22.23"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="22.98"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -232,173 +232,144 @@
       <c r="D1" s="0" t="s">
         <v>3</v>
       </c>
+      <c r="E1" s="0" t="s">
+        <v>4</v>
+      </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C2" s="0" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="D2" s="0" t="s">
-        <v>7</v>
+        <v>8</v>
+      </c>
+      <c r="E2" s="0" t="s">
+        <v>9</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="B3" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="C3" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="D3" s="0" t="s">
         <v>8</v>
       </c>
-      <c r="B3" s="0" t="s">
-        <v>9</v>
-      </c>
-      <c r="C3" s="0" t="s">
-        <v>6</v>
-      </c>
-      <c r="D3" s="0" t="s">
-        <v>7</v>
+      <c r="E3" s="0" t="s">
+        <v>9</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="C4" s="0" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="D4" s="0" t="s">
-        <v>7</v>
+        <v>8</v>
+      </c>
+      <c r="E4" s="0" t="s">
+        <v>9</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="B5" s="0" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="C5" s="0" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="D5" s="0" t="s">
-        <v>14</v>
+        <v>16</v>
+      </c>
+      <c r="E5" s="0" t="s">
+        <v>9</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="B6" s="0" t="s">
+        <v>18</v>
+      </c>
+      <c r="C6" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="D6" s="0" t="s">
         <v>16</v>
       </c>
-      <c r="C6" s="0" t="s">
-        <v>6</v>
-      </c>
-      <c r="D6" s="0" t="s">
-        <v>14</v>
+      <c r="E6" s="0" t="s">
+        <v>9</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="B7" s="0" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="C7" s="0" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="D7" s="0" t="s">
-        <v>14</v>
+        <v>16</v>
+      </c>
+      <c r="E7" s="0" t="s">
+        <v>9</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="B8" s="0" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="C8" s="0" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="D8" s="0" t="s">
-        <v>14</v>
+        <v>16</v>
+      </c>
+      <c r="E8" s="0" t="s">
+        <v>9</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="B9" s="0" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="C9" s="0" t="s">
-        <v>6</v>
-      </c>
-      <c r="D9" s="0" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="0" t="s">
-        <v>23</v>
-      </c>
-      <c r="B10" s="0" t="s">
-        <v>24</v>
-      </c>
-      <c r="C10" s="0" t="s">
-        <v>6</v>
-      </c>
-      <c r="D10" s="0" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="0" t="s">
-        <v>25</v>
-      </c>
-      <c r="B11" s="0" t="s">
-        <v>26</v>
-      </c>
-      <c r="C11" s="0" t="s">
-        <v>6</v>
-      </c>
-      <c r="D11" s="0" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="0" t="s">
-        <v>27</v>
-      </c>
-      <c r="B12" s="0" t="s">
-        <v>28</v>
-      </c>
-      <c r="C12" s="0" t="s">
-        <v>6</v>
-      </c>
-      <c r="D12" s="0" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="0" t="s">
-        <v>29</v>
-      </c>
-      <c r="B13" s="0" t="s">
-        <v>26</v>
-      </c>
-      <c r="C13" s="0" t="s">
-        <v>6</v>
-      </c>
-      <c r="D13" s="0" t="s">
-        <v>14</v>
+        <v>7</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E9" s="0" t="s">
+        <v>9</v>
       </c>
     </row>
   </sheetData>

</xml_diff>